<commit_message>
Add corncob and LMM
</commit_message>
<xml_diff>
--- a/results/outputs/qmp_sim_summ_mixed.xlsx
+++ b/results/outputs/qmp_sim_summ_mixed.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).30, 0.1 (N = 100)</t>
   </si>
@@ -24,6 +24,9 @@
     <t xml:space="preserve">LinDA.30, 0.1 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.30, 0.1 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).30, 0.2 (N = 100)</t>
   </si>
   <si>
@@ -33,6 +36,9 @@
     <t xml:space="preserve">LinDA.30, 0.2 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.30, 0.2 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).30, 0.5 (N = 100)</t>
   </si>
   <si>
@@ -42,6 +48,9 @@
     <t xml:space="preserve">LinDA.30, 0.5 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.30, 0.5 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).30, 0.9 (N = 100)</t>
   </si>
   <si>
@@ -51,6 +60,9 @@
     <t xml:space="preserve">LinDA.30, 0.9 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.30, 0.9 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).60, 0.1 (N = 100)</t>
   </si>
   <si>
@@ -60,6 +72,9 @@
     <t xml:space="preserve">LinDA.60, 0.1 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.60, 0.1 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).60, 0.2 (N = 100)</t>
   </si>
   <si>
@@ -69,6 +84,9 @@
     <t xml:space="preserve">LinDA.60, 0.2 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.60, 0.2 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).60, 0.5 (N = 100)</t>
   </si>
   <si>
@@ -78,6 +96,9 @@
     <t xml:space="preserve">LinDA.60, 0.5 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.60, 0.5 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).60, 0.9 (N = 100)</t>
   </si>
   <si>
@@ -87,6 +108,9 @@
     <t xml:space="preserve">LinDA.60, 0.9 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.60, 0.9 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).90, 0.1 (N = 100)</t>
   </si>
   <si>
@@ -96,6 +120,9 @@
     <t xml:space="preserve">LinDA.90, 0.1 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.90, 0.1 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).90, 0.2 (N = 100)</t>
   </si>
   <si>
@@ -105,6 +132,9 @@
     <t xml:space="preserve">LinDA.90, 0.2 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.90, 0.2 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).90, 0.5 (N = 100)</t>
   </si>
   <si>
@@ -114,6 +144,9 @@
     <t xml:space="preserve">LinDA.90, 0.5 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.90, 0.5 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).90, 0.9 (N = 100)</t>
   </si>
   <si>
@@ -123,6 +156,9 @@
     <t xml:space="preserve">LinDA.90, 0.9 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.90, 0.9 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).150, 0.1 (N = 100)</t>
   </si>
   <si>
@@ -132,6 +168,9 @@
     <t xml:space="preserve">LinDA.150, 0.1 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.150, 0.1 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).150, 0.2 (N = 100)</t>
   </si>
   <si>
@@ -141,6 +180,9 @@
     <t xml:space="preserve">LinDA.150, 0.2 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.150, 0.2 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).150, 0.5 (N = 100)</t>
   </si>
   <si>
@@ -150,6 +192,9 @@
     <t xml:space="preserve">LinDA.150, 0.5 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.150, 0.5 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).150, 0.9 (N = 100)</t>
   </si>
   <si>
@@ -159,6 +204,9 @@
     <t xml:space="preserve">LinDA.150, 0.9 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.150, 0.9 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).300, 0.1 (N = 100)</t>
   </si>
   <si>
@@ -168,6 +216,9 @@
     <t xml:space="preserve">LinDA.300, 0.1 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.300, 0.1 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).300, 0.2 (N = 100)</t>
   </si>
   <si>
@@ -177,6 +228,9 @@
     <t xml:space="preserve">LinDA.300, 0.2 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.300, 0.2 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).300, 0.5 (N = 100)</t>
   </si>
   <si>
@@ -186,6 +240,9 @@
     <t xml:space="preserve">LinDA.300, 0.5 (N = 100)</t>
   </si>
   <si>
+    <t xml:space="preserve">LMM-CLR.300, 0.5 (N = 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCOM-BC2 (No Filter).300, 0.9 (N = 100)</t>
   </si>
   <si>
@@ -193,6 +250,9 @@
   </si>
   <si>
     <t xml:space="preserve">LinDA.300, 0.9 (N = 100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMM-CLR.300, 0.9 (N = 100)</t>
   </si>
 </sst>
 </file>
@@ -705,6 +765,66 @@
       <c r="BH1" t="s">
         <v>59</v>
       </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -717,139 +837,139 @@
         <v>0.91</v>
       </c>
       <c r="D2" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.98</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.86</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.94</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I2" t="n">
         <v>0.98</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.85</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>0.89</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="M2" t="n">
         <v>0.97</v>
       </c>
-      <c r="K2" t="n">
+      <c r="N2" t="n">
         <v>0.85</v>
       </c>
-      <c r="L2" t="n">
+      <c r="O2" t="n">
         <v>0.76</v>
       </c>
-      <c r="M2" t="n">
+      <c r="P2" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="Q2" t="n">
         <v>1</v>
       </c>
-      <c r="N2" t="n">
+      <c r="R2" t="n">
         <v>0.91</v>
       </c>
-      <c r="O2" t="n">
+      <c r="S2" t="n">
         <v>0.98</v>
       </c>
-      <c r="P2" t="n">
+      <c r="T2" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="U2" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="V2" t="n">
         <v>0.91</v>
       </c>
-      <c r="R2" t="n">
+      <c r="W2" t="n">
         <v>0.98</v>
       </c>
-      <c r="S2" t="n">
+      <c r="X2" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="Y2" t="n">
         <v>0.99</v>
       </c>
-      <c r="T2" t="n">
+      <c r="Z2" t="n">
         <v>0.89</v>
       </c>
-      <c r="U2" t="n">
+      <c r="AA2" t="n">
         <v>0.94</v>
       </c>
-      <c r="V2" t="n">
+      <c r="AB2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AC2" t="n">
         <v>0.99</v>
       </c>
-      <c r="W2" t="n">
+      <c r="AD2" t="n">
         <v>0.92</v>
       </c>
-      <c r="X2" t="n">
+      <c r="AE2" t="n">
         <v>0.85</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="AF2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AG2" t="n">
         <v>1</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AH2" t="n">
         <v>0.93</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AI2" t="n">
         <v>0.99</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AJ2" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="AK2" t="n">
         <v>0.99</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AL2" t="n">
         <v>0.93</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AM2" t="n">
         <v>0.99</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AN2" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="AO2" t="n">
         <v>1</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AP2" t="n">
         <v>0.9</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AQ2" t="n">
         <v>0.95</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AR2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="AS2" t="n">
         <v>0.99</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AT2" t="n">
         <v>0.93</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AU2" t="n">
         <v>0.9</v>
       </c>
-      <c r="AK2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>0.96</v>
-      </c>
       <c r="AV2" t="n">
-        <v>0.93</v>
+        <v>0.84</v>
       </c>
       <c r="AW2" t="n">
         <v>1</v>
@@ -861,31 +981,91 @@
         <v>1</v>
       </c>
       <c r="AZ2" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="BA2" t="n">
         <v>1</v>
       </c>
-      <c r="BA2" t="n">
-        <v>0.96</v>
-      </c>
       <c r="BB2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="BC2" t="n">
         <v>0.99</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BD2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="BE2" t="n">
         <v>1</v>
       </c>
-      <c r="BD2" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>0.97</v>
-      </c>
       <c r="BF2" t="n">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="BG2" t="n">
         <v>0.97</v>
       </c>
       <c r="BH2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ2" t="n">
         <v>0.96</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0.95</v>
       </c>
     </row>
     <row r="3">
@@ -899,139 +1079,139 @@
         <v>0.06</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02</v>
+        <v>0.13</v>
       </c>
       <c r="E3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.03</v>
-      </c>
       <c r="G3" t="n">
         <v>0.03</v>
       </c>
       <c r="H3" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.05</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>0.04</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="M3" t="n">
         <v>0.04</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.01</v>
       </c>
       <c r="N3" t="n">
         <v>0.06</v>
       </c>
       <c r="O3" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01</v>
+        <v>0.15</v>
       </c>
       <c r="Q3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="V3" t="n">
         <v>0.05</v>
       </c>
-      <c r="R3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.02</v>
-      </c>
       <c r="W3" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="X3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AB3" t="n">
         <v>0.07</v>
       </c>
-      <c r="Y3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="Z3" t="n">
+      <c r="AC3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AH3" t="n">
         <v>0.04</v>
       </c>
-      <c r="AA3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AC3" t="n">
+      <c r="AI3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AL3" t="n">
         <v>0.04</v>
       </c>
-      <c r="AD3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AJ3" t="n">
+      <c r="AM3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AR3" t="n">
         <v>0.06</v>
       </c>
-      <c r="AK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>0.03</v>
-      </c>
       <c r="AS3" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="AT3" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="AW3" t="n">
         <v>0</v>
@@ -1043,30 +1223,90 @@
         <v>0.01</v>
       </c>
       <c r="AZ3" t="n">
-        <v>0.01</v>
+        <v>0.07</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BC3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="BI3" t="n">
         <v>0</v>
       </c>
-      <c r="BD3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BF3" t="n">
+      <c r="BJ3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="BM3" t="n">
         <v>0</v>
       </c>
-      <c r="BG3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BH3" t="n">
+      <c r="BN3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="CB3" t="n">
         <v>0.03</v>
       </c>
     </row>
@@ -1081,19 +1321,19 @@
         <v>0.25</v>
       </c>
       <c r="D4" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.07</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.04</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.14</v>
       </c>
-      <c r="G4" t="n">
-        <v>0.03</v>
-      </c>
       <c r="H4" t="n">
-        <v>0.02</v>
+        <v>0.18</v>
       </c>
       <c r="I4" t="n">
         <v>0.03</v>
@@ -1102,34 +1342,34 @@
         <v>0.02</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="L4" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O4" t="n">
         <v>0.11</v>
       </c>
-      <c r="M4" t="n">
+      <c r="P4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Q4" t="n">
         <v>0.06</v>
       </c>
-      <c r="N4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="R4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="S4" t="n">
         <v>0.42</v>
       </c>
-      <c r="P4" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.02</v>
-      </c>
       <c r="T4" t="n">
-        <v>0.01</v>
+        <v>0.64</v>
       </c>
       <c r="U4" t="n">
         <v>0.06</v>
@@ -1138,117 +1378,177 @@
         <v>0.02</v>
       </c>
       <c r="W4" t="n">
-        <v>0.01</v>
+        <v>0.26</v>
       </c>
       <c r="X4" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AE4" t="n">
         <v>0.11</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="AF4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AG4" t="n">
         <v>0.1</v>
       </c>
-      <c r="Z4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AA4" t="n">
+      <c r="AH4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AI4" t="n">
         <v>0.56</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AJ4" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AK4" t="n">
         <v>0.09</v>
       </c>
-      <c r="AC4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AD4" t="n">
+      <c r="AL4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AM4" t="n">
         <v>0.36</v>
       </c>
-      <c r="AE4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AG4" t="n">
+      <c r="AN4" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AQ4" t="n">
         <v>0.09</v>
       </c>
-      <c r="AH4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AJ4" t="n">
+      <c r="AR4" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AU4" t="n">
         <v>0.1</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AV4" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AW4" t="n">
         <v>0.12</v>
       </c>
-      <c r="AL4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AM4" t="n">
+      <c r="AX4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AY4" t="n">
         <v>0.63</v>
       </c>
-      <c r="AN4" t="n">
+      <c r="AZ4" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="BA4" t="n">
         <v>0.09</v>
       </c>
-      <c r="AO4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AP4" t="n">
+      <c r="BB4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC4" t="n">
         <v>0.42</v>
       </c>
-      <c r="AQ4" t="n">
+      <c r="BD4" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="BE4" t="n">
         <v>0.04</v>
       </c>
-      <c r="AR4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AS4" t="n">
+      <c r="BF4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BG4" t="n">
         <v>0.11</v>
       </c>
-      <c r="AT4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AU4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AV4" t="n">
+      <c r="BH4" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BK4" t="n">
         <v>0.1</v>
       </c>
-      <c r="AW4" t="n">
+      <c r="BL4" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="BM4" t="n">
         <v>0.23</v>
       </c>
-      <c r="AX4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AY4" t="n">
+      <c r="BN4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BO4" t="n">
         <v>0.72</v>
       </c>
-      <c r="AZ4" t="n">
+      <c r="BP4" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="BQ4" t="n">
         <v>0.16</v>
       </c>
-      <c r="BA4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="BB4" t="n">
+      <c r="BR4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BS4" t="n">
         <v>0.51</v>
       </c>
-      <c r="BC4" t="n">
+      <c r="BT4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="BU4" t="n">
         <v>0.06</v>
       </c>
-      <c r="BD4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BE4" t="n">
+      <c r="BV4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BW4" t="n">
         <v>0.19</v>
       </c>
-      <c r="BF4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BH4" t="n">
+      <c r="BX4" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="CB4" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -1263,175 +1563,235 @@
         <v>0.23</v>
       </c>
       <c r="D5" t="n">
-        <v>0.12</v>
+        <v>0.34</v>
       </c>
       <c r="E5" t="n">
         <v>0.12</v>
       </c>
       <c r="F5" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.14</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.05</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>0.05</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>0.04</v>
       </c>
-      <c r="J5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.02</v>
-      </c>
       <c r="L5" t="n">
-        <v>0.01</v>
+        <v>0.18</v>
       </c>
       <c r="M5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.11</v>
       </c>
-      <c r="N5" t="n">
+      <c r="R5" t="n">
         <v>0.08</v>
       </c>
-      <c r="O5" t="n">
+      <c r="S5" t="n">
         <v>0.22</v>
       </c>
-      <c r="P5" t="n">
+      <c r="T5" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="U5" t="n">
         <v>0.1</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="V5" t="n">
         <v>0.07</v>
       </c>
-      <c r="R5" t="n">
+      <c r="W5" t="n">
         <v>0.15</v>
       </c>
-      <c r="S5" t="n">
+      <c r="X5" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="Y5" t="n">
         <v>0.04</v>
       </c>
-      <c r="T5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="U5" t="n">
+      <c r="Z5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AA5" t="n">
         <v>0.05</v>
       </c>
-      <c r="V5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="Y5" t="n">
+      <c r="AB5" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AG5" t="n">
         <v>0.15</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AH5" t="n">
         <v>0.07</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AI5" t="n">
         <v>0.15</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AJ5" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="AK5" t="n">
         <v>0.13</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AL5" t="n">
         <v>0.1</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AM5" t="n">
         <v>0.12</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AN5" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="AO5" t="n">
         <v>0.04</v>
       </c>
-      <c r="AF5" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0.07</v>
-      </c>
       <c r="AP5" t="n">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="AQ5" t="n">
         <v>0.05</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.03</v>
+        <v>0.11</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="AT5" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="AU5" t="n">
         <v>0.01</v>
       </c>
       <c r="AV5" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="AW5" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="AX5" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="AY5" t="n">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="AZ5" t="n">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="BA5" t="n">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="BB5" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.02</v>
+        <v>0.16</v>
       </c>
       <c r="BE5" t="n">
         <v>0.05</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="BH5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BK5" t="n">
         <v>0</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="BT5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BU5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="BV5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BW5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="BX5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BZ5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="CA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB5" t="n">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>
@@ -1629,6 +1989,66 @@
       <c r="BH1" t="s">
         <v>59</v>
       </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1641,139 +2061,139 @@
         <v>0.9</v>
       </c>
       <c r="D2" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.98</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.86</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.93</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="I2" t="n">
         <v>0.98</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.84</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>0.89</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M2" t="n">
         <v>0.97</v>
       </c>
-      <c r="K2" t="n">
+      <c r="N2" t="n">
         <v>0.85</v>
       </c>
-      <c r="L2" t="n">
+      <c r="O2" t="n">
         <v>0.75</v>
       </c>
-      <c r="M2" t="n">
+      <c r="P2" t="n">
+        <v>0.56</v>
+      </c>
+      <c r="Q2" t="n">
         <v>1</v>
       </c>
-      <c r="N2" t="n">
+      <c r="R2" t="n">
         <v>0.91</v>
       </c>
-      <c r="O2" t="n">
+      <c r="S2" t="n">
         <v>0.98</v>
       </c>
-      <c r="P2" t="n">
+      <c r="T2" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="U2" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="V2" t="n">
         <v>0.92</v>
       </c>
-      <c r="R2" t="n">
+      <c r="W2" t="n">
         <v>0.98</v>
       </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.94</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.92</v>
-      </c>
       <c r="X2" t="n">
-        <v>0.85</v>
+        <v>0.77</v>
       </c>
       <c r="Y2" t="n">
         <v>1</v>
       </c>
       <c r="Z2" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="AA2" t="n">
         <v>0.94</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AB2" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="AC2" t="n">
         <v>0.99</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AD2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="AG2" t="n">
         <v>1</v>
       </c>
-      <c r="AC2" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="AD2" t="n">
+      <c r="AH2" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="AI2" t="n">
         <v>0.99</v>
       </c>
-      <c r="AE2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.94</v>
-      </c>
       <c r="AJ2" t="n">
-        <v>0.9</v>
+        <v>0.78</v>
       </c>
       <c r="AK2" t="n">
         <v>1</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="AM2" t="n">
         <v>0.99</v>
       </c>
       <c r="AN2" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="AO2" t="n">
         <v>1</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="AP2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AQ2" t="n">
         <v>0.95</v>
       </c>
-      <c r="AP2" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="AQ2" t="n">
+      <c r="AR2" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="AS2" t="n">
         <v>1</v>
       </c>
-      <c r="AR2" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.97</v>
-      </c>
       <c r="AT2" t="n">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.93</v>
+        <v>0.83</v>
       </c>
       <c r="AW2" t="n">
         <v>1</v>
@@ -1782,34 +2202,94 @@
         <v>0.95</v>
       </c>
       <c r="AY2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="BA2" t="n">
         <v>1</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="BB2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="BE2" t="n">
         <v>1</v>
       </c>
-      <c r="BA2" t="n">
+      <c r="BF2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ2" t="n">
         <v>0.96</v>
       </c>
-      <c r="BB2" t="n">
+      <c r="BK2" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="BS2" t="n">
         <v>0.99</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BT2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="BU2" t="n">
         <v>1</v>
       </c>
-      <c r="BD2" t="n">
+      <c r="BV2" t="n">
         <v>0.94</v>
       </c>
-      <c r="BE2" t="n">
+      <c r="BW2" t="n">
         <v>0.97</v>
       </c>
-      <c r="BF2" t="n">
+      <c r="BX2" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="BY2" t="n">
         <v>1</v>
       </c>
-      <c r="BG2" t="n">
+      <c r="BZ2" t="n">
         <v>0.96</v>
       </c>
-      <c r="BH2" t="n">
+      <c r="CA2" t="n">
         <v>0.96</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0.95</v>
       </c>
     </row>
     <row r="3">
@@ -1823,139 +2303,139 @@
         <v>0.08</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02</v>
+        <v>0.13</v>
       </c>
       <c r="E3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.07</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.04</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.03</v>
-      </c>
       <c r="H3" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.05</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>0.04</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="M3" t="n">
         <v>0.04</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.01</v>
       </c>
       <c r="N3" t="n">
         <v>0.06</v>
       </c>
       <c r="O3" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="Q3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="V3" t="n">
         <v>0.04</v>
       </c>
-      <c r="R3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.02</v>
-      </c>
       <c r="W3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AD3" t="n">
         <v>0.04</v>
       </c>
-      <c r="X3" t="n">
+      <c r="AE3" t="n">
         <v>0.07</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="AF3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="AG3" t="n">
         <v>0</v>
       </c>
-      <c r="Z3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AC3" t="n">
+      <c r="AH3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AL3" t="n">
         <v>0.04</v>
       </c>
-      <c r="AD3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AJ3" t="n">
+      <c r="AM3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AN3" t="n">
         <v>0.06</v>
       </c>
-      <c r="AK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0</v>
-      </c>
       <c r="AO3" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="AS3" t="n">
         <v>0.01</v>
       </c>
       <c r="AT3" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="AW3" t="n">
         <v>0</v>
@@ -1964,34 +2444,94 @@
         <v>0.02</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="AZ3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="BA3" t="n">
         <v>0</v>
       </c>
-      <c r="BA3" t="n">
-        <v>0.02</v>
-      </c>
       <c r="BB3" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BC3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="BE3" t="n">
         <v>0</v>
       </c>
-      <c r="BD3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>0.01</v>
-      </c>
       <c r="BF3" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="BH3" t="n">
         <v>0.03</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>0.02</v>
       </c>
     </row>
     <row r="4">
@@ -2005,91 +2545,91 @@
         <v>0.25</v>
       </c>
       <c r="D4" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.07</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.03</v>
-      </c>
       <c r="F4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.14</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.04</v>
       </c>
-      <c r="H4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.03</v>
-      </c>
       <c r="J4" t="n">
         <v>0.02</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="L4" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O4" t="n">
         <v>0.11</v>
       </c>
-      <c r="M4" t="n">
+      <c r="P4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="Q4" t="n">
         <v>0.06</v>
       </c>
-      <c r="N4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="R4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="S4" t="n">
         <v>0.37</v>
       </c>
-      <c r="P4" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.02</v>
-      </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="U4" t="n">
         <v>0.05</v>
       </c>
       <c r="V4" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="W4" t="n">
-        <v>0.01</v>
+        <v>0.21</v>
       </c>
       <c r="X4" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AE4" t="n">
         <v>0.11</v>
       </c>
-      <c r="Y4" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0.03</v>
-      </c>
       <c r="AF4" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="AG4" t="n">
         <v>0.08</v>
@@ -2098,81 +2638,141 @@
         <v>0.02</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.01</v>
+        <v>0.51</v>
       </c>
       <c r="AJ4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AU4" t="n">
         <v>0.1</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AV4" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AW4" t="n">
         <v>0.11</v>
       </c>
-      <c r="AL4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AM4" t="n">
+      <c r="AX4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AY4" t="n">
         <v>0.6</v>
       </c>
-      <c r="AN4" t="n">
+      <c r="AZ4" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="BA4" t="n">
         <v>0.09</v>
       </c>
-      <c r="AO4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AP4" t="n">
+      <c r="BB4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC4" t="n">
         <v>0.4</v>
       </c>
-      <c r="AQ4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AS4" t="n">
+      <c r="BD4" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BG4" t="n">
         <v>0.11</v>
       </c>
-      <c r="AT4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AU4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AV4" t="n">
+      <c r="BH4" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BK4" t="n">
         <v>0.1</v>
       </c>
-      <c r="AW4" t="n">
+      <c r="BL4" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="BM4" t="n">
         <v>0.19</v>
       </c>
-      <c r="AX4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AY4" t="n">
+      <c r="BN4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BO4" t="n">
         <v>0.71</v>
       </c>
-      <c r="AZ4" t="n">
+      <c r="BP4" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="BQ4" t="n">
         <v>0.13</v>
       </c>
-      <c r="BA4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BB4" t="n">
+      <c r="BR4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BS4" t="n">
         <v>0.5</v>
       </c>
-      <c r="BC4" t="n">
+      <c r="BT4" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="BU4" t="n">
         <v>0.05</v>
       </c>
-      <c r="BD4" t="n">
+      <c r="BV4" t="n">
         <v>0</v>
       </c>
-      <c r="BE4" t="n">
+      <c r="BW4" t="n">
         <v>0.18</v>
       </c>
-      <c r="BF4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BH4" t="n">
+      <c r="BX4" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="CB4" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -2187,175 +2787,235 @@
         <v>0.23</v>
       </c>
       <c r="D5" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.13</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.11</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>0.14</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.07</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>0.07</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>0.04</v>
       </c>
-      <c r="J5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.02</v>
-      </c>
       <c r="L5" t="n">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="M5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.13</v>
       </c>
-      <c r="N5" t="n">
+      <c r="R5" t="n">
         <v>0.09</v>
       </c>
-      <c r="O5" t="n">
+      <c r="S5" t="n">
         <v>0.22</v>
       </c>
-      <c r="P5" t="n">
+      <c r="T5" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="U5" t="n">
         <v>0.09</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="V5" t="n">
         <v>0.06</v>
       </c>
-      <c r="R5" t="n">
+      <c r="W5" t="n">
         <v>0.15</v>
       </c>
-      <c r="S5" t="n">
+      <c r="X5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Y5" t="n">
         <v>0.04</v>
       </c>
-      <c r="T5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="U5" t="n">
+      <c r="Z5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AA5" t="n">
         <v>0.04</v>
       </c>
-      <c r="V5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="Y5" t="n">
+      <c r="AB5" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AG5" t="n">
         <v>0.14</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AH5" t="n">
         <v>0.09</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AI5" t="n">
         <v>0.17</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AJ5" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="AK5" t="n">
         <v>0.12</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AL5" t="n">
         <v>0.1</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0.08</v>
       </c>
       <c r="AM5" t="n">
         <v>0.13</v>
       </c>
       <c r="AN5" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="BA5" t="n">
         <v>0.11</v>
       </c>
-      <c r="AO5" t="n">
+      <c r="BB5" t="n">
         <v>0.08</v>
       </c>
-      <c r="AP5" t="n">
+      <c r="BC5" t="n">
         <v>0.11</v>
       </c>
-      <c r="AQ5" t="n">
+      <c r="BD5" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="BE5" t="n">
         <v>0.04</v>
       </c>
-      <c r="AR5" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AS5" t="n">
+      <c r="BF5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BG5" t="n">
         <v>0.06</v>
       </c>
-      <c r="AT5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AV5" t="n">
+      <c r="BH5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BK5" t="n">
         <v>0</v>
       </c>
-      <c r="AW5" t="n">
+      <c r="BL5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BM5" t="n">
         <v>0.17</v>
       </c>
-      <c r="AX5" t="n">
+      <c r="BN5" t="n">
         <v>0.07</v>
       </c>
-      <c r="AY5" t="n">
+      <c r="BO5" t="n">
         <v>0.05</v>
       </c>
-      <c r="AZ5" t="n">
+      <c r="BP5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BQ5" t="n">
         <v>0.11</v>
       </c>
-      <c r="BA5" t="n">
+      <c r="BR5" t="n">
         <v>0.06</v>
       </c>
-      <c r="BB5" t="n">
+      <c r="BS5" t="n">
         <v>0.05</v>
       </c>
-      <c r="BC5" t="n">
+      <c r="BT5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="BU5" t="n">
         <v>0.04</v>
       </c>
-      <c r="BD5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BE5" t="n">
+      <c r="BV5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BW5" t="n">
         <v>0.06</v>
       </c>
-      <c r="BF5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BH5" t="n">
+      <c r="BX5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BZ5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="CA5" t="n">
         <v>0</v>
+      </c>
+      <c r="CB5" t="n">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>